<commit_message>
PGD works with no variable load
</commit_message>
<xml_diff>
--- a/Codi/PGD/data_10PQ.xlsx
+++ b/Codi/PGD/data_10PQ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josep\Desktop\CITCEA\Codi\PGD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840D6276-8BD2-41D2-82CE-4FCFDC92C067}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18908D19-6BBA-4939-8D12-3196077D2D78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{43544277-89E4-4F72-87F2-FECA9F9384A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43544277-89E4-4F72-87F2-FECA9F9384A7}"/>
   </bookViews>
   <sheets>
     <sheet name="buses" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A9F03E-3FB2-47D9-B81B-D17612DC601D}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -533,7 +533,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -557,7 +557,7 @@
       </c>
       <c r="B6">
         <f>B5</f>
-        <v>-0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:G13" si="0">C5</f>
@@ -586,7 +586,7 @@
       </c>
       <c r="B7">
         <f t="shared" ref="B7:B13" si="1">B6</f>
-        <v>-0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -615,7 +615,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>-0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -644,7 +644,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>-0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -673,7 +673,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>-0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="1"/>
-        <v>-0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -731,7 +731,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="1"/>
-        <v>-0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -760,7 +760,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="1"/>
-        <v>-0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -792,7 +792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAEDE02B-082B-43FE-958E-56326AECD5D3}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>